<commit_message>
Base bar plot for Fig 1 panel B, still need to match to IPCC bibliography
</commit_message>
<xml_diff>
--- a/R/factor_aesthetics.xlsx
+++ b/R/factor_aesthetics.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="23">
   <si>
     <t>label</t>
   </si>
@@ -61,6 +61,33 @@
   </si>
   <si>
     <t>level</t>
+  </si>
+  <si>
+    <t>oro_type</t>
+  </si>
+  <si>
+    <t>Marine renewable energy</t>
+  </si>
+  <si>
+    <t>CO2 removal or storage</t>
+  </si>
+  <si>
+    <t>Increase efficiency</t>
+  </si>
+  <si>
+    <t>Human assisted evolution</t>
+  </si>
+  <si>
+    <t>Conservation</t>
+  </si>
+  <si>
+    <t>Built infrastructure &amp; technology</t>
+  </si>
+  <si>
+    <t>Socio-institutional</t>
+  </si>
+  <si>
+    <t>Human-assisted evolution</t>
   </si>
 </sst>
 </file>
@@ -378,15 +405,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="13.36328125" customWidth="1"/>
+    <col min="3" max="3" width="16.453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
@@ -457,7 +485,134 @@
         <v>12</v>
       </c>
     </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5" t="str">
+        <f>E2</f>
+        <v>#35a7d9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6">
+        <v>2</v>
+      </c>
+      <c r="E6" t="str">
+        <f>E2</f>
+        <v>#35a7d9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7">
+        <v>3</v>
+      </c>
+      <c r="E7" t="str">
+        <f>E2</f>
+        <v>#35a7d9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8">
+        <v>4</v>
+      </c>
+      <c r="E8" t="str">
+        <f>E3</f>
+        <v>forestgreen</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9">
+        <v>5</v>
+      </c>
+      <c r="E9" t="str">
+        <f>E3</f>
+        <v>forestgreen</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10">
+        <v>6</v>
+      </c>
+      <c r="E10" t="str">
+        <f>E4</f>
+        <v>#7670a8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11">
+        <v>7</v>
+      </c>
+      <c r="E11" t="str">
+        <f>E4</f>
+        <v>#7670a8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Plot figure 3 as a simple stacked barplot of method types as a proportion of all predicted articles for each oro type
</commit_message>
<xml_diff>
--- a/R/factor_aesthetics.xlsx
+++ b/R/factor_aesthetics.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="34">
   <si>
     <t>label</t>
   </si>
@@ -88,6 +88,39 @@
   </si>
   <si>
     <t>Human-assisted evolution</t>
+  </si>
+  <si>
+    <t>method_type</t>
+  </si>
+  <si>
+    <t>Mathematical_predictionsimulation</t>
+  </si>
+  <si>
+    <t>Social_primary</t>
+  </si>
+  <si>
+    <t>Empirical</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>Social primary</t>
+  </si>
+  <si>
+    <t>Prediction/simulation</t>
+  </si>
+  <si>
+    <t>#1b9e77</t>
+  </si>
+  <si>
+    <t>#d95f02</t>
+  </si>
+  <si>
+    <t>#7570b3</t>
+  </si>
+  <si>
+    <t>darkgrey</t>
   </si>
 </sst>
 </file>
@@ -405,10 +438,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -611,6 +644,74 @@
         <v>#7670a8</v>
       </c>
     </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" t="s">
+        <v>26</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" t="s">
+        <v>28</v>
+      </c>
+      <c r="D13">
+        <v>2</v>
+      </c>
+      <c r="E13" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D14">
+        <v>3</v>
+      </c>
+      <c r="E14" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" t="s">
+        <v>27</v>
+      </c>
+      <c r="D15">
+        <v>4</v>
+      </c>
+      <c r="E15" t="s">
+        <v>33</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Try plotting panel B as a heatmap, but I find we lose the presentation of the gradient in types of OROs deployed across the marine systems.
</commit_message>
<xml_diff>
--- a/R/factor_aesthetics.xlsx
+++ b/R/factor_aesthetics.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="49">
   <si>
     <t>label</t>
   </si>
@@ -121,6 +121,51 @@
   </si>
   <si>
     <t>darkgrey</t>
+  </si>
+  <si>
+    <t>marine_system</t>
+  </si>
+  <si>
+    <t>Coastal land</t>
+  </si>
+  <si>
+    <t>Coastal ocean</t>
+  </si>
+  <si>
+    <t>Open-ocean</t>
+  </si>
+  <si>
+    <t>climate_threat</t>
+  </si>
+  <si>
+    <t>Temperature</t>
+  </si>
+  <si>
+    <t>SLR</t>
+  </si>
+  <si>
+    <t>Extreme_weather</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>Sea level rise</t>
+  </si>
+  <si>
+    <t>Extreme weather</t>
+  </si>
+  <si>
+    <t>land</t>
+  </si>
+  <si>
+    <t>open_ocean</t>
+  </si>
+  <si>
+    <t>coastal_ocean</t>
+  </si>
+  <si>
+    <t>Unidentified</t>
   </si>
 </sst>
 </file>
@@ -438,10 +483,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -712,6 +757,125 @@
         <v>33</v>
       </c>
     </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>34</v>
+      </c>
+      <c r="B16" t="s">
+        <v>45</v>
+      </c>
+      <c r="C16" t="s">
+        <v>35</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>34</v>
+      </c>
+      <c r="B17" t="s">
+        <v>47</v>
+      </c>
+      <c r="C17" t="s">
+        <v>36</v>
+      </c>
+      <c r="D17">
+        <v>2</v>
+      </c>
+      <c r="E17" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" t="s">
+        <v>46</v>
+      </c>
+      <c r="C18" t="s">
+        <v>37</v>
+      </c>
+      <c r="D18">
+        <v>3</v>
+      </c>
+      <c r="E18" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>38</v>
+      </c>
+      <c r="B19" t="s">
+        <v>39</v>
+      </c>
+      <c r="C19" t="s">
+        <v>39</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="E19" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>38</v>
+      </c>
+      <c r="B20" t="s">
+        <v>40</v>
+      </c>
+      <c r="C20" t="s">
+        <v>43</v>
+      </c>
+      <c r="D20">
+        <v>2</v>
+      </c>
+      <c r="E20" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>38</v>
+      </c>
+      <c r="B21" t="s">
+        <v>41</v>
+      </c>
+      <c r="C21" t="s">
+        <v>44</v>
+      </c>
+      <c r="D21">
+        <v>3</v>
+      </c>
+      <c r="E21" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>38</v>
+      </c>
+      <c r="B22" t="s">
+        <v>42</v>
+      </c>
+      <c r="C22" t="s">
+        <v>48</v>
+      </c>
+      <c r="D22">
+        <v>4</v>
+      </c>
+      <c r="E22" t="s">
+        <v>42</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Not sure how to plot panel B, so code chunks for different options
</commit_message>
<xml_diff>
--- a/R/factor_aesthetics.xlsx
+++ b/R/factor_aesthetics.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="53">
   <si>
     <t>label</t>
   </si>
@@ -166,6 +166,18 @@
   </si>
   <si>
     <t>Unidentified</t>
+  </si>
+  <si>
+    <t>#DC267F</t>
+  </si>
+  <si>
+    <t>#648FFF</t>
+  </si>
+  <si>
+    <t>#FE6100</t>
+  </si>
+  <si>
+    <t>#5D5C5E</t>
   </si>
 </sst>
 </file>
@@ -486,7 +498,7 @@
   <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -822,7 +834,7 @@
         <v>1</v>
       </c>
       <c r="E19" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
@@ -839,7 +851,7 @@
         <v>2</v>
       </c>
       <c r="E20" t="s">
-        <v>42</v>
+        <v>50</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
@@ -856,7 +868,7 @@
         <v>3</v>
       </c>
       <c r="E21" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
@@ -873,7 +885,7 @@
         <v>4</v>
       </c>
       <c r="E22" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
draft plot C.i for mitigation, and make notes for further investigation (absence of salt marsh, MRE x coral reef in mitigation outcomes)
</commit_message>
<xml_diff>
--- a/R/factor_aesthetics.xlsx
+++ b/R/factor_aesthetics.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="67">
   <si>
     <t>label</t>
   </si>
@@ -178,6 +178,48 @@
   </si>
   <si>
     <t>#5D5C5E</t>
+  </si>
+  <si>
+    <t>ecosystem_type</t>
+  </si>
+  <si>
+    <t>Salt_marsh</t>
+  </si>
+  <si>
+    <t>Mangrove</t>
+  </si>
+  <si>
+    <t>Coral_reef</t>
+  </si>
+  <si>
+    <t>Seagrass</t>
+  </si>
+  <si>
+    <t>Salt marsh</t>
+  </si>
+  <si>
+    <t>Coral reef</t>
+  </si>
+  <si>
+    <t>#E69F00</t>
+  </si>
+  <si>
+    <t>#009E73</t>
+  </si>
+  <si>
+    <t>#56B4E9</t>
+  </si>
+  <si>
+    <t>#D55E00</t>
+  </si>
+  <si>
+    <t>adapt_to_threat</t>
+  </si>
+  <si>
+    <t>Human</t>
+  </si>
+  <si>
+    <t>Natural</t>
   </si>
 </sst>
 </file>
@@ -495,10 +537,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -888,6 +930,102 @@
         <v>52</v>
       </c>
     </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>53</v>
+      </c>
+      <c r="B23" t="s">
+        <v>54</v>
+      </c>
+      <c r="C23" t="s">
+        <v>58</v>
+      </c>
+      <c r="D23">
+        <v>1</v>
+      </c>
+      <c r="E23" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>53</v>
+      </c>
+      <c r="B24" t="s">
+        <v>55</v>
+      </c>
+      <c r="C24" t="s">
+        <v>55</v>
+      </c>
+      <c r="D24">
+        <v>2</v>
+      </c>
+      <c r="E24" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>53</v>
+      </c>
+      <c r="B25" t="s">
+        <v>57</v>
+      </c>
+      <c r="C25" t="s">
+        <v>57</v>
+      </c>
+      <c r="D25">
+        <v>3</v>
+      </c>
+      <c r="E25" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>53</v>
+      </c>
+      <c r="B26" t="s">
+        <v>56</v>
+      </c>
+      <c r="C26" t="s">
+        <v>59</v>
+      </c>
+      <c r="D26">
+        <v>4</v>
+      </c>
+      <c r="E26" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>64</v>
+      </c>
+      <c r="B27" t="s">
+        <v>65</v>
+      </c>
+      <c r="C27" t="s">
+        <v>65</v>
+      </c>
+      <c r="D27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>64</v>
+      </c>
+      <c r="B28" t="s">
+        <v>66</v>
+      </c>
+      <c r="C28" t="s">
+        <v>6</v>
+      </c>
+      <c r="D28">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
modification of hex codes for ORO types
</commit_message>
<xml_diff>
--- a/R/factor_aesthetics.xlsx
+++ b/R/factor_aesthetics.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20405"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03EC2F66-F190-424D-9B3A-0E7A8821B874}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="74">
   <si>
     <t>label</t>
   </si>
@@ -220,12 +221,33 @@
   </si>
   <si>
     <t>Natural</t>
+  </si>
+  <si>
+    <t>#026996</t>
+  </si>
+  <si>
+    <t>#0688c2</t>
+  </si>
+  <si>
+    <t>#9ed7f0</t>
+  </si>
+  <si>
+    <t>#43b08a</t>
+  </si>
+  <si>
+    <t>#078257</t>
+  </si>
+  <si>
+    <t>#600787</t>
+  </si>
+  <si>
+    <t>#ad5ad1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -536,20 +558,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="13.36328125" customWidth="1"/>
-    <col min="3" max="3" width="16.453125" customWidth="1"/>
+    <col min="1" max="1" width="13.6640625" customWidth="1"/>
+    <col min="2" max="2" width="31.77734375" customWidth="1"/>
+    <col min="3" max="3" width="16.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -566,7 +589,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -583,7 +606,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -600,7 +623,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -617,7 +640,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -630,12 +653,11 @@
       <c r="D5">
         <v>1</v>
       </c>
-      <c r="E5" t="str">
-        <f>E2</f>
-        <v>#35a7d9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E5" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -648,12 +670,11 @@
       <c r="D6">
         <v>2</v>
       </c>
-      <c r="E6" t="str">
-        <f>E2</f>
-        <v>#35a7d9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E6" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -666,12 +687,11 @@
       <c r="D7">
         <v>3</v>
       </c>
-      <c r="E7" t="str">
-        <f>E2</f>
-        <v>#35a7d9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E7" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -684,12 +704,11 @@
       <c r="D8">
         <v>4</v>
       </c>
-      <c r="E8" t="str">
-        <f>E3</f>
-        <v>forestgreen</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E8" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -702,12 +721,11 @@
       <c r="D9">
         <v>5</v>
       </c>
-      <c r="E9" t="str">
-        <f>E3</f>
-        <v>forestgreen</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E9" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -720,12 +738,11 @@
       <c r="D10">
         <v>6</v>
       </c>
-      <c r="E10" t="str">
-        <f>E4</f>
-        <v>#7670a8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E10" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -738,12 +755,11 @@
       <c r="D11">
         <v>7</v>
       </c>
-      <c r="E11" t="str">
-        <f>E4</f>
-        <v>#7670a8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E11" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>23</v>
       </c>
@@ -760,7 +776,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>23</v>
       </c>
@@ -777,7 +793,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>23</v>
       </c>
@@ -794,7 +810,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>23</v>
       </c>
@@ -811,7 +827,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>34</v>
       </c>
@@ -828,7 +844,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>34</v>
       </c>
@@ -845,7 +861,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>34</v>
       </c>
@@ -862,7 +878,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>38</v>
       </c>
@@ -879,7 +895,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>38</v>
       </c>
@@ -896,7 +912,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>38</v>
       </c>
@@ -913,7 +929,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>38</v>
       </c>
@@ -930,7 +946,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>53</v>
       </c>
@@ -947,7 +963,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>53</v>
       </c>
@@ -964,7 +980,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>53</v>
       </c>
@@ -981,7 +997,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>53</v>
       </c>
@@ -998,7 +1014,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>64</v>
       </c>
@@ -1012,7 +1028,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>64</v>
       </c>

</xml_diff>

<commit_message>
Update fig 1 to include policy moments and different colours for ORO types
</commit_message>
<xml_diff>
--- a/R/factor_aesthetics.xlsx
+++ b/R/factor_aesthetics.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="74">
   <si>
     <t>label</t>
   </si>
@@ -220,6 +220,27 @@
   </si>
   <si>
     <t>Natural</t>
+  </si>
+  <si>
+    <t>#026996</t>
+  </si>
+  <si>
+    <t>#0688c2</t>
+  </si>
+  <si>
+    <t>#9ed7f0</t>
+  </si>
+  <si>
+    <t>#078257</t>
+  </si>
+  <si>
+    <t>#43b08a</t>
+  </si>
+  <si>
+    <t>#600787</t>
+  </si>
+  <si>
+    <t>#ad5ad1</t>
   </si>
 </sst>
 </file>
@@ -539,8 +560,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -630,9 +651,8 @@
       <c r="D5">
         <v>1</v>
       </c>
-      <c r="E5" t="str">
-        <f>E2</f>
-        <v>#35a7d9</v>
+      <c r="E5" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
@@ -648,9 +668,8 @@
       <c r="D6">
         <v>2</v>
       </c>
-      <c r="E6" t="str">
-        <f>E2</f>
-        <v>#35a7d9</v>
+      <c r="E6" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
@@ -666,9 +685,8 @@
       <c r="D7">
         <v>3</v>
       </c>
-      <c r="E7" t="str">
-        <f>E2</f>
-        <v>#35a7d9</v>
+      <c r="E7" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
@@ -676,17 +694,16 @@
         <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C8" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D8">
         <v>4</v>
       </c>
-      <c r="E8" t="str">
-        <f>E3</f>
-        <v>forestgreen</v>
+      <c r="E8" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
@@ -694,17 +711,16 @@
         <v>14</v>
       </c>
       <c r="B9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C9" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D9">
         <v>5</v>
       </c>
-      <c r="E9" t="str">
-        <f>E3</f>
-        <v>forestgreen</v>
+      <c r="E9" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
@@ -720,9 +736,8 @@
       <c r="D10">
         <v>6</v>
       </c>
-      <c r="E10" t="str">
-        <f>E4</f>
-        <v>#7670a8</v>
+      <c r="E10" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
@@ -738,9 +753,8 @@
       <c r="D11">
         <v>7</v>
       </c>
-      <c r="E11" t="str">
-        <f>E4</f>
-        <v>#7670a8</v>
+      <c r="E11" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
make hovmoller plot of outcome type % contribution to each ORO type by year
</commit_message>
<xml_diff>
--- a/R/factor_aesthetics.xlsx
+++ b/R/factor_aesthetics.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="80">
   <si>
     <t>label</t>
   </si>
@@ -241,6 +241,24 @@
   </si>
   <si>
     <t>#ad5ad1</t>
+  </si>
+  <si>
+    <t>Human adaptation</t>
+  </si>
+  <si>
+    <t>Natural adaptation</t>
+  </si>
+  <si>
+    <t>#33a02c</t>
+  </si>
+  <si>
+    <t>#b2df8a</t>
+  </si>
+  <si>
+    <t>#1f78b4</t>
+  </si>
+  <si>
+    <t>outcome_type</t>
   </si>
 </sst>
 </file>
@@ -558,10 +576,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E28"/>
+  <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1040,6 +1058,57 @@
         <v>2</v>
       </c>
     </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>79</v>
+      </c>
+      <c r="B29" t="s">
+        <v>5</v>
+      </c>
+      <c r="C29" t="s">
+        <v>5</v>
+      </c>
+      <c r="D29">
+        <v>1</v>
+      </c>
+      <c r="E29" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>79</v>
+      </c>
+      <c r="B30" t="s">
+        <v>75</v>
+      </c>
+      <c r="C30" t="s">
+        <v>75</v>
+      </c>
+      <c r="D30">
+        <v>2</v>
+      </c>
+      <c r="E30" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>79</v>
+      </c>
+      <c r="B31" t="s">
+        <v>74</v>
+      </c>
+      <c r="C31" t="s">
+        <v>74</v>
+      </c>
+      <c r="D31">
+        <v>3</v>
+      </c>
+      <c r="E31" t="s">
+        <v>76</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
modify methods plots so two empirical study types are grouped, model F1 appears in legend, and supplemental hovmoller plot is configured so dark colours = high articles
</commit_message>
<xml_diff>
--- a/R/factor_aesthetics.xlsx
+++ b/R/factor_aesthetics.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="78">
   <si>
     <t>label</t>
   </si>
@@ -105,21 +105,9 @@
     <t>Other</t>
   </si>
   <si>
-    <t>Social primary</t>
-  </si>
-  <si>
     <t>Prediction/simulation</t>
   </si>
   <si>
-    <t>#1b9e77</t>
-  </si>
-  <si>
-    <t>#d95f02</t>
-  </si>
-  <si>
-    <t>#7570b3</t>
-  </si>
-  <si>
     <t>darkgrey</t>
   </si>
   <si>
@@ -259,6 +247,12 @@
   </si>
   <si>
     <t>outcome_type</t>
+  </si>
+  <si>
+    <t>Empirical - other</t>
+  </si>
+  <si>
+    <t>Empirical - social primary</t>
   </si>
 </sst>
 </file>
@@ -578,12 +572,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="K23" sqref="K23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
+    <col min="1" max="1" width="17.1796875" customWidth="1"/>
     <col min="2" max="2" width="13.36328125" customWidth="1"/>
     <col min="3" max="3" width="16.453125" customWidth="1"/>
   </cols>
@@ -670,7 +665,7 @@
         <v>1</v>
       </c>
       <c r="E5" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
@@ -687,7 +682,7 @@
         <v>2</v>
       </c>
       <c r="E6" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
@@ -704,7 +699,7 @@
         <v>3</v>
       </c>
       <c r="E7" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
@@ -721,7 +716,7 @@
         <v>4</v>
       </c>
       <c r="E8" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
@@ -738,7 +733,7 @@
         <v>5</v>
       </c>
       <c r="E9" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
@@ -755,7 +750,7 @@
         <v>6</v>
       </c>
       <c r="E10" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
@@ -772,7 +767,7 @@
         <v>7</v>
       </c>
       <c r="E11" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
@@ -783,13 +778,13 @@
         <v>26</v>
       </c>
       <c r="C12" t="s">
-        <v>26</v>
+        <v>76</v>
       </c>
       <c r="D12">
         <v>1</v>
       </c>
       <c r="E12" t="s">
-        <v>30</v>
+        <v>72</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
@@ -800,13 +795,13 @@
         <v>25</v>
       </c>
       <c r="C13" t="s">
-        <v>28</v>
+        <v>77</v>
       </c>
       <c r="D13">
         <v>2</v>
       </c>
       <c r="E13" t="s">
-        <v>31</v>
+        <v>73</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
@@ -817,13 +812,13 @@
         <v>24</v>
       </c>
       <c r="C14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D14">
         <v>3</v>
       </c>
       <c r="E14" t="s">
-        <v>32</v>
+        <v>74</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
@@ -840,205 +835,205 @@
         <v>4</v>
       </c>
       <c r="E15" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B16" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C16" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="D16">
         <v>1</v>
       </c>
       <c r="E16" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B17" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C17" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D17">
         <v>2</v>
       </c>
       <c r="E17" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B18" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C18" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="D18">
         <v>3</v>
       </c>
       <c r="E18" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B19" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C19" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D19">
         <v>1</v>
       </c>
       <c r="E19" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B20" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C20" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="D20">
         <v>2</v>
       </c>
       <c r="E20" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B21" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C21" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D21">
         <v>3</v>
       </c>
       <c r="E21" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
+        <v>34</v>
+      </c>
+      <c r="B22" t="s">
         <v>38</v>
       </c>
-      <c r="B22" t="s">
-        <v>42</v>
-      </c>
       <c r="C22" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="D22">
         <v>4</v>
       </c>
       <c r="E22" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B23" t="s">
+        <v>50</v>
+      </c>
+      <c r="C23" t="s">
         <v>54</v>
-      </c>
-      <c r="C23" t="s">
-        <v>58</v>
       </c>
       <c r="D23">
         <v>1</v>
       </c>
       <c r="E23" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B24" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C24" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="D24">
         <v>2</v>
       </c>
       <c r="E24" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
+        <v>49</v>
+      </c>
+      <c r="B25" t="s">
         <v>53</v>
       </c>
-      <c r="B25" t="s">
-        <v>57</v>
-      </c>
       <c r="C25" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D25">
         <v>3</v>
       </c>
       <c r="E25" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B26" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C26" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="D26">
         <v>4</v>
       </c>
       <c r="E26" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B27" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C27" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D27">
         <v>1</v>
@@ -1046,10 +1041,10 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B28" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C28" t="s">
         <v>6</v>
@@ -1060,7 +1055,7 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B29" t="s">
         <v>5</v>
@@ -1072,41 +1067,41 @@
         <v>1</v>
       </c>
       <c r="E29" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B30" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C30" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="D30">
         <v>2</v>
       </c>
       <c r="E30" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B31" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C31" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D31">
         <v>3</v>
       </c>
       <c r="E31" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>